<commit_message>
Updated with NSE values
</commit_message>
<xml_diff>
--- a/mendota/FreshFiles-from-2019-11-20/PQT/Simulations/NSE_RMSE_Values.xlsx
+++ b/mendota/FreshFiles-from-2019-11-20/PQT/Simulations/NSE_RMSE_Values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patriciatran/Documents/GLM955-South/mendota/FreshFiles-from-2019-11-20/PQT/Simulations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7934F3F7-56FF-1449-A84B-212E12D410C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E1ADD8-3113-AA40-8079-FAB3F4A54BDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{F70A4C78-8B65-9A45-A9BD-33F7CC588364}"/>
   </bookViews>
@@ -424,13 +424,13 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -465,6 +465,9 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
+      <c r="B4">
+        <v>0.95688099999999998</v>
+      </c>
       <c r="C4">
         <v>1.319</v>
       </c>

</xml_diff>

<commit_message>
Updated the scenarios and code to make figures
</commit_message>
<xml_diff>
--- a/mendota/FreshFiles-from-2019-11-20/PQT/Simulations/NSE_RMSE_Values.xlsx
+++ b/mendota/FreshFiles-from-2019-11-20/PQT/Simulations/NSE_RMSE_Values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patriciatran/Documents/GLM955-South/mendota/FreshFiles-from-2019-11-20/PQT/Simulations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E1ADD8-3113-AA40-8079-FAB3F4A54BDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02F56D3-3AD4-8F4B-927A-DDC03A4FD1C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{F70A4C78-8B65-9A45-A9BD-33F7CC588364}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>Scenario</t>
   </si>
@@ -52,6 +52,30 @@
   </si>
   <si>
     <t>A3</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>No salt</t>
+  </si>
+  <si>
+    <t>Constant salt value of 0.1</t>
+  </si>
+  <si>
+    <t>Constant salt value of 01</t>
+  </si>
+  <si>
+    <t>Constant salt value of 10</t>
+  </si>
+  <si>
+    <t>Lake</t>
+  </si>
+  <si>
+    <t>Mendota</t>
+  </si>
+  <si>
+    <t>Monona</t>
   </si>
 </sst>
 </file>
@@ -104,9 +128,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,63 +447,147 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F6A709-A14E-DB4C-8E88-0951119D1366}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2">
+        <v>0.95792560000000004</v>
+      </c>
+      <c r="D2">
         <v>1.3029999999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3">
+        <v>0.95488709999999999</v>
+      </c>
+      <c r="D3">
         <v>1.349</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>0.95688099999999998</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>1.319</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5">
+        <v>0.8830692</v>
+      </c>
+      <c r="D5">
         <v>2.1720000000000002</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Temp plots surface and bottom changed :-)
</commit_message>
<xml_diff>
--- a/mendota/FreshFiles-from-2019-11-20/PQT/Simulations/NSE_RMSE_Values.xlsx
+++ b/mendota/FreshFiles-from-2019-11-20/PQT/Simulations/NSE_RMSE_Values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patriciatran/Documents/GLM955-South/mendota/FreshFiles-from-2019-11-20/PQT/Simulations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02F56D3-3AD4-8F4B-927A-DDC03A4FD1C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FF5DFA-213C-8340-8EC3-43787E6C3208}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{F70A4C78-8B65-9A45-A9BD-33F7CC588364}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{F70A4C78-8B65-9A45-A9BD-33F7CC588364}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>Scenario</t>
   </si>
@@ -75,7 +75,34 @@
     <t>Mendota</t>
   </si>
   <si>
-    <t>Monona</t>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>Constant salt value of 35</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>Constant salt value of 0.1, then drop to 0 in 2010</t>
+  </si>
+  <si>
+    <t>Constant salt value of 10, then drop to 0 in 2010</t>
+  </si>
+  <si>
+    <t>Constant salt value of 35, then drop to 0 in 2010</t>
+  </si>
+  <si>
+    <t>Constant salt value of 1, then drop to 0 in 2010</t>
   </si>
 </sst>
 </file>
@@ -447,7 +474,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F6A709-A14E-DB4C-8E88-0951119D1366}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
@@ -489,7 +516,7 @@
         <v>0.95792560000000004</v>
       </c>
       <c r="D2">
-        <v>1.3029999999999999</v>
+        <v>1.3</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
@@ -506,7 +533,7 @@
         <v>0.95488709999999999</v>
       </c>
       <c r="D3">
-        <v>1.349</v>
+        <v>1.35</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -523,7 +550,7 @@
         <v>0.95688099999999998</v>
       </c>
       <c r="D4">
-        <v>1.319</v>
+        <v>1.32</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -540,7 +567,7 @@
         <v>0.8830692</v>
       </c>
       <c r="D5">
-        <v>2.1720000000000002</v>
+        <v>2.17</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
@@ -548,49 +575,91 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>3</v>
+      <c r="C6">
+        <v>0.81043200000000004</v>
+      </c>
+      <c r="D6">
+        <v>2.77</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>0.95328029999999997</v>
+      </c>
+      <c r="D7">
+        <v>1.37</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>0.95716210000000002</v>
+      </c>
+      <c r="D8">
+        <v>1.31</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>0.84670400000000001</v>
+      </c>
+      <c r="D9">
+        <v>2.4900000000000002</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>0.45768249999999999</v>
+      </c>
+      <c r="D10">
+        <v>4.68</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>